<commit_message>
Manual corrections: ER, FVG
</commit_message>
<xml_diff>
--- a/external/correzioni/MAR.xlsx
+++ b/external/correzioni/MAR.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidenicoli/Local_Workspace/TesiMag/Riunioni/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidenicoli/Local_Workspace/TesiMag/external/correzioni/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4999EAE0-A045-494A-A840-A6E31E7FE515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22FAEBC4-11A1-4942-8AE2-463939893EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20480" windowHeight="12800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="merged" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2187" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2187" uniqueCount="432">
   <si>
     <t>sensor_key</t>
   </si>
@@ -1310,6 +1310,12 @@
   </si>
   <si>
     <t>controllare merging con san benedetto</t>
+  </si>
+  <si>
+    <t>lon_ok</t>
+  </si>
+  <si>
+    <t>lat_ok</t>
   </si>
 </sst>
 </file>
@@ -2164,9 +2170,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="75" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A136" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AD153" sqref="AD153"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="75" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2279,10 +2285,10 @@
         <v>25</v>
       </c>
       <c r="AA1" s="2" t="s">
-        <v>13</v>
+        <v>430</v>
       </c>
       <c r="AB1" s="2" t="s">
-        <v>14</v>
+        <v>431</v>
       </c>
       <c r="AC1" s="2" t="s">
         <v>384</v>

</xml_diff>

<commit_message>
Correzioni manuali MAR e LOM
</commit_message>
<xml_diff>
--- a/external/correzioni/MAR.xlsx
+++ b/external/correzioni/MAR.xlsx
@@ -1,26 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidenicoli/Local_Workspace/TesiMag/external/correzioni/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22FAEBC4-11A1-4942-8AE2-463939893EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{847EA213-081E-8546-A08D-45C3F70D1E33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="merged" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">merged!$A$1:$AD$165</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2187" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2185" uniqueCount="430">
   <si>
     <t>sensor_key</t>
   </si>
@@ -1304,12 +1307,6 @@
   </si>
   <si>
     <t>è in Umbria?</t>
-  </si>
-  <si>
-    <t>controllare merging con SAB BENEDETTO DEL TRONTO</t>
-  </si>
-  <si>
-    <t>controllare merging con san benedetto</t>
   </si>
   <si>
     <t>lon_ok</t>
@@ -1829,7 +1826,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1847,6 +1844,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Colore 1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2170,9 +2172,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="75" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AB2" sqref="AB2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K137" sqref="K137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2285,10 +2287,10 @@
         <v>25</v>
       </c>
       <c r="AA1" s="2" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="AB1" s="2" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="AC1" s="2" t="s">
         <v>384</v>
@@ -12895,179 +12897,170 @@
         <v>37</v>
       </c>
     </row>
-    <row r="128" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A128" s="4">
+    <row r="128" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A128" s="11">
         <v>373</v>
       </c>
-      <c r="B128" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C128" s="4">
+      <c r="B128" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C128" s="11">
         <v>120</v>
       </c>
-      <c r="D128" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E128" s="4" t="s">
+      <c r="D128" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E128" s="11" t="s">
         <v>330</v>
       </c>
-      <c r="F128" s="4" t="s">
+      <c r="F128" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="G128" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H128" s="4" t="s">
+      <c r="G128" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H128" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="I128" s="4" t="s">
+      <c r="I128" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="J128" s="4" t="s">
+      <c r="J128" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="K128" s="4">
+      <c r="K128" s="11">
         <v>11140</v>
       </c>
-      <c r="L128" s="4">
+      <c r="L128" s="11">
         <v>120</v>
       </c>
-      <c r="M128" s="4" t="s">
+      <c r="M128" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="N128" s="4">
+      <c r="N128" s="11">
         <v>13.889167</v>
       </c>
-      <c r="O128" s="4">
+      <c r="O128" s="11">
         <v>42.933224000000003</v>
       </c>
-      <c r="P128" s="4">
+      <c r="P128" s="11">
         <v>2</v>
       </c>
-      <c r="Q128" s="4">
+      <c r="Q128" s="11">
         <v>4.4360766410827601</v>
       </c>
-      <c r="R128" s="4">
+      <c r="R128" s="11">
         <v>10663</v>
       </c>
-      <c r="S128" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="T128" s="4" t="s">
+      <c r="S128" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="T128" s="11" t="s">
         <v>331</v>
       </c>
-      <c r="U128" s="4" t="s">
+      <c r="U128" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="V128" s="5">
+      <c r="V128" s="12">
         <v>37910</v>
       </c>
-      <c r="W128" s="5">
+      <c r="W128" s="12">
         <v>45291</v>
       </c>
-      <c r="X128" s="4">
+      <c r="X128" s="11">
         <v>7129</v>
       </c>
-      <c r="Y128" s="4">
+      <c r="Y128" s="11">
         <v>7129</v>
       </c>
-      <c r="Z128" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA128" s="4"/>
-      <c r="AB128" s="4"/>
-      <c r="AC128" s="4">
+      <c r="Z128" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC128" s="11">
         <v>6</v>
       </c>
-      <c r="AD128" s="6" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="129" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A129" s="4">
+      <c r="AD128" s="13"/>
+    </row>
+    <row r="129" spans="1:30" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="11">
         <v>372</v>
       </c>
-      <c r="B129" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C129" s="4">
+      <c r="B129" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C129" s="11">
         <v>2913</v>
       </c>
-      <c r="D129" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E129" s="4" t="s">
+      <c r="D129" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E129" s="11" t="s">
         <v>329</v>
       </c>
-      <c r="F129" s="4" t="s">
+      <c r="F129" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="G129" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H129" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I129" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J129" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K129" s="4">
+      <c r="G129" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H129" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I129" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="J129" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="K129" s="11">
         <v>70033</v>
       </c>
-      <c r="L129" s="4">
+      <c r="L129" s="11">
         <v>2913</v>
       </c>
-      <c r="M129" s="4" t="s">
+      <c r="M129" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="N129" s="4">
+      <c r="N129" s="11">
         <v>13.889799999999999</v>
       </c>
-      <c r="O129" s="4">
+      <c r="O129" s="11">
         <v>42.955100000000002</v>
       </c>
-      <c r="P129" s="4">
+      <c r="P129" s="11">
         <v>0</v>
       </c>
-      <c r="Q129" s="4">
+      <c r="Q129" s="11">
         <v>0</v>
       </c>
-      <c r="R129" s="4">
+      <c r="R129" s="11">
         <v>6940</v>
       </c>
-      <c r="S129" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="T129" s="4">
+      <c r="S129" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="T129" s="11">
         <v>3494</v>
       </c>
-      <c r="U129" s="4" t="s">
+      <c r="U129" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="V129" s="5">
+      <c r="V129" s="12">
         <v>40348</v>
       </c>
-      <c r="W129" s="5">
+      <c r="W129" s="12">
         <v>44926</v>
       </c>
-      <c r="X129" s="4">
+      <c r="X129" s="11">
         <v>3716</v>
       </c>
-      <c r="Y129" s="4">
+      <c r="Y129" s="11">
         <v>3716</v>
       </c>
-      <c r="Z129" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA129" s="4"/>
-      <c r="AB129" s="4"/>
-      <c r="AC129" s="4"/>
-      <c r="AD129" s="6" t="s">
-        <v>429</v>
-      </c>
+      <c r="Z129" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD129" s="13"/>
     </row>
     <row r="130" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A130">
@@ -13661,7 +13654,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="137" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A137" s="4">
         <v>382</v>
       </c>
@@ -13740,12 +13733,9 @@
       <c r="Z137" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AA137" s="4"/>
-      <c r="AB137" s="4"/>
-      <c r="AC137" s="4"/>
       <c r="AD137" s="6"/>
     </row>
-    <row r="138" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A138" s="4">
         <v>381</v>
       </c>
@@ -13824,8 +13814,6 @@
       <c r="Z138" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AA138" s="4"/>
-      <c r="AB138" s="4"/>
       <c r="AC138" s="4">
         <v>386</v>
       </c>
@@ -16108,6 +16096,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AD165" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AD165">
     <sortCondition ref="E2:E165"/>
   </sortState>

</xml_diff>